<commit_message>
turned the excel file into csvs to put in as langchain docs
</commit_message>
<xml_diff>
--- a/Data/SMU FAQs.xlsx
+++ b/Data/SMU FAQs.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yawbt\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yawbt\OneDrive\Documents\GitHub\SURF-Project_Optimizing-PerunaBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0D41380B-1960-426B-BAC6-F4C06850695F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D740EFEE-EB26-4882-B4F9-6112CE01B685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{536CA00E-8293-4F5E-AC4F-99F4811B1994}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{536CA00E-8293-4F5E-AC4F-99F4811B1994}"/>
   </bookViews>
   <sheets>
-    <sheet name="SMU FAQs" sheetId="1" r:id="rId1"/>
+    <sheet name="University Advising Center FAQs" sheetId="1" r:id="rId1"/>
     <sheet name="Student Financial Services FAQs" sheetId="2" r:id="rId2"/>
     <sheet name="Parent FAQs" sheetId="3" r:id="rId3"/>
     <sheet name="SMU Experience FAQs" sheetId="4" r:id="rId4"/>
@@ -1471,6 +1471,69 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1524,6 +1587,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1531,105 +1603,7 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -1659,8 +1633,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1675,35 +1653,39 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1776,6 +1758,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1784,18 +1782,20 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
+        <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -1812,44 +1812,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0922651F-4840-434A-AFCD-7C32AE8C0F85}" name="Table1" displayName="Table1" ref="A2:B31" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0922651F-4840-434A-AFCD-7C32AE8C0F85}" name="Table1" displayName="Table1" ref="A2:B31" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A2:B31" xr:uid="{0922651F-4840-434A-AFCD-7C32AE8C0F85}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{272DA8E4-69E0-4C65-91FF-E0508F4F00B6}" name="question" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FA0DDA33-07F1-4040-BF1A-5D91EB839E7B}" name=" answer" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{272DA8E4-69E0-4C65-91FF-E0508F4F00B6}" name="question" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{FA0DDA33-07F1-4040-BF1A-5D91EB839E7B}" name=" answer" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A980924B-B78B-47CF-86C7-0302FFDC464B}" name="Table2" displayName="Table2" ref="A2:B38" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A980924B-B78B-47CF-86C7-0302FFDC464B}" name="Table2" displayName="Table2" ref="A2:B38" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A2:B38" xr:uid="{A980924B-B78B-47CF-86C7-0302FFDC464B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7E295157-9265-4556-A6FE-83E52492FA07}" name="question" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{1FC6FA69-1B2C-4FCF-8BD8-03D1BA985184}" name="answer" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{7E295157-9265-4556-A6FE-83E52492FA07}" name="question" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1FC6FA69-1B2C-4FCF-8BD8-03D1BA985184}" name="answer" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{82BAAC23-C0B7-4663-8FD0-A6DDAD5AE868}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{82BAAC23-C0B7-4663-8FD0-A6DDAD5AE868}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A2:B9" xr:uid="{82BAAC23-C0B7-4663-8FD0-A6DDAD5AE868}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A4232353-1732-4CB1-B92C-92C4628047A9}" name="question" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{EB4DB9CF-F6AF-4556-83A0-378C8921EA69}" name="answer" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{A4232353-1732-4CB1-B92C-92C4628047A9}" name="question" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{EB4DB9CF-F6AF-4556-83A0-378C8921EA69}" name="answer" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03E11441-AABB-4399-B01A-F5A323EABA11}" name="Table4" displayName="Table4" ref="A2:B14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03E11441-AABB-4399-B01A-F5A323EABA11}" name="Table4" displayName="Table4" ref="A2:B14" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A2:B14" xr:uid="{03E11441-AABB-4399-B01A-F5A323EABA11}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3170B6FE-5778-4234-BB0A-DEC943AEDB51}" name="question" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{7BB91E8F-DE1C-435D-B3BE-FBD5CA70DA3C}" name="answer" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3170B6FE-5778-4234-BB0A-DEC943AEDB51}" name="question" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7BB91E8F-DE1C-435D-B3BE-FBD5CA70DA3C}" name="answer" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2174,7 +2174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B6148D-E968-4543-B099-0CAAF3497845}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2444,8 +2444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6794590-A6EB-472C-BFFC-D317237830BB}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2477,7 +2477,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>64</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>68</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>69</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>70</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>71</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>73</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="377" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>77</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>82</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>84</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>85</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>87</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>89</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>91</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>93</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>95</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>98</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>99</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>100</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>101</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>105</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>108</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>110</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>111</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>113</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>153</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>163</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>173</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>176</v>
       </c>

</xml_diff>

<commit_message>
wrote code for base OpenAI model gpt_4o and tested the three retrievers/vectorstores
</commit_message>
<xml_diff>
--- a/Data/SMU FAQs.xlsx
+++ b/Data/SMU FAQs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yawbt\OneDrive\Documents\GitHub\SURF-Project_Optimizing-PerunaBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D740EFEE-EB26-4882-B4F9-6112CE01B685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E9E8AD-4F00-4CC6-888B-2A0B0FE8D954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{536CA00E-8293-4F5E-AC4F-99F4811B1994}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{536CA00E-8293-4F5E-AC4F-99F4811B1994}"/>
   </bookViews>
   <sheets>
     <sheet name="University Advising Center FAQs" sheetId="1" r:id="rId1"/>
@@ -1402,11 +1402,8 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1469,7 +1466,96 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="30">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1812,44 +1898,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0922651F-4840-434A-AFCD-7C32AE8C0F85}" name="Table1" displayName="Table1" ref="A2:B31" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0922651F-4840-434A-AFCD-7C32AE8C0F85}" name="Table1" displayName="Table1" ref="A2:B31" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A2:B31" xr:uid="{0922651F-4840-434A-AFCD-7C32AE8C0F85}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{272DA8E4-69E0-4C65-91FF-E0508F4F00B6}" name="question" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{FA0DDA33-07F1-4040-BF1A-5D91EB839E7B}" name=" answer" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{272DA8E4-69E0-4C65-91FF-E0508F4F00B6}" name="question" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{FA0DDA33-07F1-4040-BF1A-5D91EB839E7B}" name=" answer" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A980924B-B78B-47CF-86C7-0302FFDC464B}" name="Table2" displayName="Table2" ref="A2:B38" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A980924B-B78B-47CF-86C7-0302FFDC464B}" name="Table2" displayName="Table2" ref="A2:B38" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="A2:B38" xr:uid="{A980924B-B78B-47CF-86C7-0302FFDC464B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7E295157-9265-4556-A6FE-83E52492FA07}" name="question" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{1FC6FA69-1B2C-4FCF-8BD8-03D1BA985184}" name="answer" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{7E295157-9265-4556-A6FE-83E52492FA07}" name="question" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1FC6FA69-1B2C-4FCF-8BD8-03D1BA985184}" name="answer" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{82BAAC23-C0B7-4663-8FD0-A6DDAD5AE868}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{82BAAC23-C0B7-4663-8FD0-A6DDAD5AE868}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A2:B9" xr:uid="{82BAAC23-C0B7-4663-8FD0-A6DDAD5AE868}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A4232353-1732-4CB1-B92C-92C4628047A9}" name="question" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{EB4DB9CF-F6AF-4556-83A0-378C8921EA69}" name="answer" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A4232353-1732-4CB1-B92C-92C4628047A9}" name="question" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{EB4DB9CF-F6AF-4556-83A0-378C8921EA69}" name="answer" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03E11441-AABB-4399-B01A-F5A323EABA11}" name="Table4" displayName="Table4" ref="A2:B14" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D1E82172-009B-4B96-825E-DCFCB9CB213B}" name="Table5" displayName="Table5" ref="A2:B23" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="A2:B23" xr:uid="{D1E82172-009B-4B96-825E-DCFCB9CB213B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{42157492-80BE-4371-B671-C004401400FC}" name="question" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2C96D280-17AD-46EE-8095-0E6EA745A764}" name="answer" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{03E11441-AABB-4399-B01A-F5A323EABA11}" name="Table4" displayName="Table4" ref="A2:B14" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A2:B14" xr:uid="{03E11441-AABB-4399-B01A-F5A323EABA11}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3170B6FE-5778-4234-BB0A-DEC943AEDB51}" name="question" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{7BB91E8F-DE1C-435D-B3BE-FBD5CA70DA3C}" name="answer" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3170B6FE-5778-4234-BB0A-DEC943AEDB51}" name="question" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7BB91E8F-DE1C-435D-B3BE-FBD5CA70DA3C}" name="answer" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2174,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B6148D-E968-4543-B099-0CAAF3497845}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2185,247 +2282,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2444,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6794590-A6EB-472C-BFFC-D317237830BB}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2462,298 +2559,298 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="145" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2769,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E46768-3E54-4882-9A45-F554D63C4CD1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2785,66 +2882,66 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="116" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2860,7 +2957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1148FC8-BC70-4D6D-9E57-38041AC895AF}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A18" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2874,183 +2973,186 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>192</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3059,7 +3161,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3074,106 +3176,106 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>